<commit_message>
Finalized Sprint 2 & Sprint 1 comments
</commit_message>
<xml_diff>
--- a/Team5Report.xlsx
+++ b/Team5Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StevensUser\Documents\GitHub\SSW555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02319A90-927D-46D5-9FCD-ED916B19F643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{65FD6749-57B4-4F10-8245-38489CD3CA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="275">
   <si>
     <t>Initials</t>
   </si>
@@ -722,9 +722,6 @@
     <t>Compare birth and marriage</t>
   </si>
   <si>
-    <t>coding</t>
-  </si>
-  <si>
     <t>not started</t>
   </si>
   <si>
@@ -843,6 +840,35 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue to communicate effectively </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop user stories by seperating into
+separate tasks </t>
+  </si>
+  <si>
+    <t>Use numpy to format our charts</t>
+  </si>
+  <si>
+    <t>Not starting the sprint ahead of time</t>
+  </si>
+  <si>
+    <t>Not solving issues with original code 
+before beginning new user stories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ready for development </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Less then 150 years old </t>
+  </si>
+  <si>
+    <t>Unique ID's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique Name and Birth Date </t>
   </si>
 </sst>
 </file>
@@ -983,7 +1009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1033,6 +1059,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1328,6 +1357,9 @@
                 <c:pt idx="0">
                   <c:v>44829</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>44837</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1339,6 +1371,9 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2198,10 +2233,10 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1114425" cy="628650"/>
+    <xdr:ext cx="1114425" cy="901700"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Shape 3">
@@ -2215,8 +2250,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4793550" y="3470438"/>
-          <a:ext cx="1104900" cy="619125"/>
+          <a:off x="1352550" y="1174750"/>
+          <a:ext cx="1114425" cy="901700"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -2306,10 +2341,10 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1104900" cy="533400"/>
+    <xdr:ext cx="1104900" cy="806450"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="Shape 4">
@@ -2323,8 +2358,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4798313" y="3518063"/>
-          <a:ext cx="1095375" cy="523875"/>
+          <a:off x="5680075" y="1155700"/>
+          <a:ext cx="1104900" cy="806450"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -3103,7 +3138,7 @@
         <v>189</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4124,8 +4159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4193,7 +4228,7 @@
         <v>191</v>
       </c>
       <c r="E2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -4215,7 +4250,7 @@
         <v>191</v>
       </c>
       <c r="E3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -4236,8 +4271,8 @@
       <c r="D4" t="s">
         <v>193</v>
       </c>
-      <c r="E4" t="s">
-        <v>226</v>
+      <c r="E4" s="17" t="s">
+        <v>265</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -4257,8 +4292,8 @@
       <c r="D5" t="s">
         <v>193</v>
       </c>
-      <c r="E5" t="s">
-        <v>227</v>
+      <c r="E5" s="17" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4275,7 +4310,7 @@
         <v>190</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4292,7 +4327,7 @@
         <v>192</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4303,13 +4338,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>192</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4326,7 +4361,7 @@
         <v>190</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4343,7 +4378,7 @@
         <v>191</v>
       </c>
       <c r="E10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4360,7 +4395,7 @@
         <v>191</v>
       </c>
       <c r="E11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4371,13 +4406,13 @@
         <v>68</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>190</v>
       </c>
       <c r="E12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4388,13 +4423,13 @@
         <v>82</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>190</v>
       </c>
       <c r="E13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4405,13 +4440,13 @@
         <v>76</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>192</v>
       </c>
       <c r="E14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4422,13 +4457,13 @@
         <v>79</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>192</v>
       </c>
       <c r="E15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4445,7 +4480,7 @@
         <v>193</v>
       </c>
       <c r="E16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4462,7 +4497,7 @@
         <v>193</v>
       </c>
       <c r="E17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4479,7 +4514,7 @@
         <v>191</v>
       </c>
       <c r="E18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4496,7 +4531,7 @@
         <v>191</v>
       </c>
       <c r="E19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4513,7 +4548,7 @@
         <v>192</v>
       </c>
       <c r="E20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4524,13 +4559,13 @@
         <v>157</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>192</v>
       </c>
       <c r="E21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4541,13 +4576,13 @@
         <v>160</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>190</v>
       </c>
       <c r="E22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4558,13 +4593,13 @@
         <v>15</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>190</v>
       </c>
       <c r="E23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4581,7 +4616,7 @@
         <v>193</v>
       </c>
       <c r="E24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4598,7 +4633,7 @@
         <v>193</v>
       </c>
       <c r="E25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4609,13 +4644,13 @@
         <v>85</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>191</v>
       </c>
       <c r="E26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4632,7 +4667,7 @@
         <v>191</v>
       </c>
       <c r="E27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4643,13 +4678,13 @@
         <v>103</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>190</v>
       </c>
       <c r="E28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4660,13 +4695,13 @@
         <v>94</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>190</v>
       </c>
       <c r="E29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4677,13 +4712,13 @@
         <v>97</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>192</v>
       </c>
       <c r="E30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4694,13 +4729,13 @@
         <v>100</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>192</v>
       </c>
       <c r="E31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4717,7 +4752,7 @@
         <v>193</v>
       </c>
       <c r="E32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4734,13 +4769,13 @@
         <v>193</v>
       </c>
       <c r="E33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B35" s="29"/>
       <c r="C35" s="29"/>
@@ -4751,7 +4786,7 @@
         <v>91</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4759,7 +4794,7 @@
         <v>106</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4767,7 +4802,7 @@
         <v>118</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4775,7 +4810,7 @@
         <v>121</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4783,7 +4818,7 @@
         <v>124</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4791,7 +4826,7 @@
         <v>127</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4799,7 +4834,7 @@
         <v>130</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4807,7 +4842,7 @@
         <v>136</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4815,7 +4850,7 @@
         <v>166</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4823,7 +4858,7 @@
         <v>169</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5795,7 +5830,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5941,7 +5978,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" ref="D16:D19" si="0">C15-C16</f>
+        <f>C15-C16</f>
         <v>6</v>
       </c>
       <c r="E16" s="9">
@@ -5951,7 +5988,7 @@
         <v>120</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" ref="G16:G19" si="1">(E16-E15)/F16*60</f>
+        <f>(E16-E15)/F16*60</f>
         <v>125.00000000000001</v>
       </c>
     </row>
@@ -5966,7 +6003,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D16:D19" si="0">C16-C17</f>
         <v>6</v>
       </c>
       <c r="E17" s="9">
@@ -5976,7 +6013,7 @@
         <v>135</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G16:G19" si="1">(E17-E16)/F17*60</f>
         <v>102.22222222222223</v>
       </c>
     </row>
@@ -9966,7 +10003,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10033,12 +10070,26 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="5"/>
+      <c r="A3" s="4">
+        <v>44837</v>
+      </c>
+      <c r="B3" s="2">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2">
+        <f>B2-B3</f>
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>92</v>
+      </c>
+      <c r="E3" s="2">
+        <v>200</v>
+      </c>
+      <c r="F3" s="5">
+        <f>(D3-D2)/E3*60</f>
+        <v>27.6</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -14039,8 +14090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14112,7 +14163,7 @@
         <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14121,7 +14172,7 @@
         <v>195</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>190</v>
@@ -14135,7 +14186,7 @@
         <v>196</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>190</v>
@@ -14149,7 +14200,7 @@
         <v>197</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>190</v>
@@ -14185,7 +14236,7 @@
         <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14258,7 +14309,7 @@
         <v>60</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14340,7 +14391,7 @@
         <v>20</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14351,7 +14402,7 @@
         <v>205</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>192</v>
@@ -14366,7 +14417,7 @@
         <v>206</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>192</v>
@@ -14381,7 +14432,7 @@
         <v>207</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C24" s="28" t="s">
         <v>192</v>
@@ -14393,10 +14444,10 @@
     </row>
     <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>192</v>
@@ -14408,10 +14459,10 @@
     </row>
     <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>192</v>
@@ -14450,7 +14501,7 @@
         <v>20</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14532,7 +14583,7 @@
         <v>30</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14543,7 +14594,7 @@
         <v>202</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>190</v>
@@ -14558,7 +14609,7 @@
         <v>203</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>190</v>
@@ -14573,7 +14624,7 @@
         <v>204</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>190</v>
@@ -14606,7 +14657,15 @@
       <c r="F40">
         <v>55</v>
       </c>
-      <c r="I40" s="27"/>
+      <c r="G40">
+        <v>12</v>
+      </c>
+      <c r="H40">
+        <v>60</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I41" s="27"/>
@@ -14710,7 +14769,15 @@
       <c r="F48">
         <v>45</v>
       </c>
-      <c r="I48" s="27"/>
+      <c r="G48">
+        <v>15</v>
+      </c>
+      <c r="H48">
+        <v>65</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="49" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="23"/>
@@ -14813,28 +14880,40 @@
       </c>
       <c r="I59" s="27"/>
     </row>
-    <row r="60" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="3"/>
+    <row r="60" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="3" t="s">
+        <v>266</v>
+      </c>
       <c r="I60" s="27"/>
     </row>
-    <row r="61" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="3"/>
+    <row r="61" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="3" t="s">
+        <v>267</v>
+      </c>
       <c r="I61" s="27"/>
     </row>
-    <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="3"/>
+    <row r="62" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="3" t="s">
+        <v>268</v>
+      </c>
       <c r="I62" s="27"/>
     </row>
-    <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="11" t="s">
         <v>53</v>
       </c>
       <c r="I63" s="27"/>
     </row>
-    <row r="64" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="3" t="s">
+        <v>269</v>
+      </c>
       <c r="I64" s="27"/>
     </row>
-    <row r="65" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="30" t="s">
+        <v>270</v>
+      </c>
       <c r="I65" s="27"/>
     </row>
     <row r="66" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -18591,13 +18670,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="26" width="10.69140625" customWidth="1"/>
+    <col min="1" max="1" width="10.69140625" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="8.3046875" customWidth="1"/>
+    <col min="4" max="4" width="22.07421875" customWidth="1"/>
+    <col min="5" max="26" width="10.69140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -18629,21 +18712,173 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>35</v>
+      </c>
+    </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+    </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+    </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
+    </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" t="s">
+        <v>271</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>75</v>
+      </c>
+    </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>60</v>
+      </c>
+    </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" t="s">
+        <v>271</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>55</v>
+      </c>
+    </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" t="s">
+        <v>271</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>45</v>
+      </c>
+    </row>
     <row r="17" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -19632,7 +19867,7 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21730,8 +21965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
User story 10 and 11
</commit_message>
<xml_diff>
--- a/Team5Report.xlsx
+++ b/Team5Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frank\Documents\CS 555\SSW555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\SSW555Group\SSW555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0B52C1-AECF-4557-844A-87D6D66C5272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D4DA40-DD7B-43B4-8839-0A03C56525E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="275">
   <si>
     <t>Initials</t>
   </si>
@@ -14090,7 +14090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
@@ -18671,7 +18671,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18761,6 +18761,15 @@
       <c r="F4">
         <v>30</v>
       </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18781,6 +18790,15 @@
       </c>
       <c r="F6">
         <v>30</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>40</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -21992,8 +22010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed user story for sprint 3
</commit_message>
<xml_diff>
--- a/Team5Report.xlsx
+++ b/Team5Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frank\Documents\CS 555\SSW555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14343B20-782A-45B0-8628-CBDF063D388F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E129FC5-2E9E-447D-88F1-4B46BE2CA1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="275">
   <si>
     <t>Initials</t>
   </si>
@@ -866,6 +866,9 @@
   </si>
   <si>
     <t>Refactor and keep code organized</t>
+  </si>
+  <si>
+    <t>No more than 15 siblings</t>
   </si>
 </sst>
 </file>
@@ -4170,8 +4173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20012,7 +20015,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20055,10 +20058,10 @@
     </row>
     <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>77</v>
+        <v>274</v>
       </c>
       <c r="C2" t="s">
         <v>190</v>
@@ -22297,8 +22300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>